<commit_message>
Including some sheets for analysis; and correlation analysis code for parameters of sammons and t-sne;
</commit_message>
<xml_diff>
--- a/PaperNeural/ResultGraphs/best_and_worse_acc.xlsx
+++ b/PaperNeural/ResultGraphs/best_and_worse_acc.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oliveirafhm/Dropbox/Compartilhada Alessando e Fabio/Clinic 09.03.2016/Programs/oliveirafhm/code_paper_journal_2017/PaperNeural/ResultGraphs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oliveirafhm/OneDrive/Doutorado/Compartilhada_Alessando_Fabio/Clinic 09.03.2016/Programs/oliveirafhm/code_paper_journal_2017/PaperNeural/ResultGraphs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-1900" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AC$177</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AD$177</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -30,18 +30,18 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Fábio Henrique Monteiro Oliveira</author>
   </authors>
   <commentList>
-    <comment ref="Z1" authorId="0">
+    <comment ref="Z1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
@@ -50,23 +50,41 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-1 - Best
-2 - Worst</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">1 - Best
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>2 - Worst</t>
         </r>
       </text>
     </comment>
-    <comment ref="AA1" authorId="0">
+    <comment ref="AA1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
@@ -75,23 +93,41 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-1 - CV set acc
-2 - Test set acc</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">1 - CV set acc
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>2 - Test set acc</t>
         </r>
       </text>
     </comment>
-    <comment ref="AB1" authorId="0">
+    <comment ref="AB1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
@@ -100,12 +136,21 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-(CVMAcc + TestSetAcc) / 2</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>(CVMAcc + TestSetAcc) / 2</t>
         </r>
       </text>
     </comment>
@@ -114,7 +159,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1433" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1434" uniqueCount="419">
   <si>
     <t>PaperNeural</t>
   </si>
@@ -1368,12 +1413,15 @@
   </si>
   <si>
     <t>InFigure</t>
+  </si>
+  <si>
+    <t>QR_STD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1405,15 +1453,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="10"/>
-      <color indexed="81"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
-      <b/>
       <sz val="10"/>
-      <color indexed="81"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1445,7 +1493,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1461,6 +1509,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1741,14 +1791,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:AC177"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:AD177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q1" sqref="Q1"/>
-      <selection pane="bottomLeft" activeCell="W4" sqref="W4"/>
+      <selection pane="bottomLeft" activeCell="AB68" sqref="AB68:AB110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1775,15 +1825,16 @@
     <col min="21" max="21" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="70.5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="44.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="44.6640625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="8.5" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.1640625" customWidth="1"/>
+    <col min="30" max="30" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1869,10 +1920,13 @@
         <v>416</v>
       </c>
       <c r="AC1" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="AD1" s="1" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="2" spans="1:29" s="8" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -1955,11 +2009,15 @@
         <v>1</v>
       </c>
       <c r="AB2" s="8">
-        <f t="shared" ref="AB2:AB33" si="0">AVERAGE(U2:V2)</f>
+        <f>AVERAGE(U2:V2)</f>
         <v>68.713450292397667</v>
       </c>
+      <c r="AC2" s="8">
+        <f>_xlfn.STDEV.S(U2:V2)</f>
+        <v>15.299971288831689</v>
+      </c>
     </row>
-    <row r="3" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2042,11 +2100,15 @@
         <v>1</v>
       </c>
       <c r="AB3" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="AB3:AB5" si="0">AVERAGE(U3:V3)</f>
         <v>69.005847953216374</v>
       </c>
+      <c r="AC3" s="8">
+        <f t="shared" ref="AC3:AC66" si="1">_xlfn.STDEV.S(U3:V3)</f>
+        <v>0.82702547507197877</v>
+      </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>6</v>
       </c>
@@ -2128,15 +2190,19 @@
       <c r="AA4">
         <v>2</v>
       </c>
-      <c r="AB4" s="8">
-        <f t="shared" si="0"/>
+      <c r="AB4" s="13">
+        <f>AVERAGE(U4:V4)</f>
         <v>79.824561403508767</v>
       </c>
-      <c r="AC4">
+      <c r="AC4" s="13">
+        <f>_xlfn.STDEV.S(U4:V4)</f>
+        <v>6.2026910630398957</v>
+      </c>
+      <c r="AD4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>7</v>
       </c>
@@ -2219,11 +2285,15 @@
         <v>2</v>
       </c>
       <c r="AB5" s="8">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(U5:V5)</f>
         <v>67.251461988304101</v>
       </c>
+      <c r="AC5" s="8">
+        <f>_xlfn.STDEV.S(U5:V5)</f>
+        <v>13.232407601151779</v>
+      </c>
     </row>
-    <row r="6" spans="1:29" s="8" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
         <v>11</v>
       </c>
@@ -2309,8 +2379,12 @@
         <f>AVERAGE(U6:V6)</f>
         <v>80.994152046783626</v>
       </c>
+      <c r="AC6" s="8">
+        <f>_xlfn.STDEV.S(U6:V6)</f>
+        <v>10.337818438399809</v>
+      </c>
     </row>
-    <row r="7" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>12</v>
       </c>
@@ -2396,25 +2470,29 @@
         <f>AVERAGE(U7:V7)</f>
         <v>61.403508771929829</v>
       </c>
+      <c r="AC7" s="8">
+        <f>_xlfn.STDEV.S(U7:V7)</f>
+        <v>4.9621528504319024</v>
+      </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>14</v>
+        <v>510</v>
       </c>
       <c r="B8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8">
-        <v>-1</v>
+        <v>3000</v>
       </c>
       <c r="F8">
-        <v>-1</v>
+        <v>0.6</v>
       </c>
       <c r="G8">
         <v>-1</v>
@@ -2441,53 +2519,57 @@
         <v>1</v>
       </c>
       <c r="O8" t="s">
-        <v>89</v>
+        <v>403</v>
       </c>
       <c r="P8">
-        <v>-1</v>
-      </c>
-      <c r="Q8">
-        <v>-1</v>
+        <v>575</v>
+      </c>
+      <c r="Q8" s="14">
+        <v>4.9107899495603409E-2</v>
       </c>
       <c r="R8">
-        <v>-1</v>
+        <v>58</v>
       </c>
       <c r="S8">
-        <v>-1</v>
+        <v>14.013008146414252</v>
       </c>
       <c r="T8">
-        <v>-1</v>
+        <v>0.97633724382374631</v>
       </c>
       <c r="U8">
-        <v>83.040935672514621</v>
+        <v>82.456140350877192</v>
       </c>
       <c r="V8">
-        <v>89.473684210526315</v>
+        <v>94.736842105263165</v>
       </c>
       <c r="W8" t="s">
-        <v>90</v>
+        <v>404</v>
       </c>
       <c r="X8" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="Y8" s="12">
-        <v>7</v>
-      </c>
-      <c r="Z8">
-        <v>1</v>
-      </c>
-      <c r="AA8">
-        <v>2</v>
-      </c>
-      <c r="AB8" s="8">
+        <v>30</v>
+      </c>
+      <c r="Z8" s="5">
+        <v>1</v>
+      </c>
+      <c r="AA8" s="5">
+        <v>2</v>
+      </c>
+      <c r="AB8" s="13">
         <f>AVERAGE(U8:V8)</f>
-        <v>86.257309941520475</v>
-      </c>
-      <c r="AC8">
+        <v>88.596491228070178</v>
+      </c>
+      <c r="AC8" s="13">
+        <f>_xlfn.STDEV.S(U8:V8)</f>
+        <v>8.6837674882558531</v>
+      </c>
+      <c r="AD8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>12</v>
       </c>
@@ -2573,8 +2655,12 @@
         <f>AVERAGE(U9:V9)</f>
         <v>61.403508771929829</v>
       </c>
+      <c r="AC9" s="8">
+        <f>_xlfn.STDEV.S(U9:V9)</f>
+        <v>4.9621528504319024</v>
+      </c>
     </row>
-    <row r="10" spans="1:29" s="8" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8">
         <v>17</v>
       </c>
@@ -2660,8 +2746,12 @@
         <f>AVERAGE(U10:V10)</f>
         <v>73.684210526315795</v>
       </c>
+      <c r="AC10" s="8">
+        <f>_xlfn.STDEV.S(U10:V10)</f>
+        <v>7.4432292756478597</v>
+      </c>
     </row>
-    <row r="11" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>16</v>
       </c>
@@ -2747,28 +2837,32 @@
         <f>AVERAGE(U11:V11)</f>
         <v>57.894736842105267</v>
       </c>
+      <c r="AC11" s="8">
+        <f>_xlfn.STDEV.S(U11:V11)</f>
+        <v>14.88645855129573</v>
+      </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>20</v>
+        <v>2665</v>
       </c>
       <c r="B12">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E12">
-        <v>-1</v>
+        <v>5000</v>
       </c>
       <c r="F12">
-        <v>-1</v>
+        <v>600</v>
       </c>
       <c r="G12">
-        <v>-1</v>
+        <v>27.5</v>
       </c>
       <c r="H12" t="s">
         <v>0</v>
@@ -2792,53 +2886,57 @@
         <v>1</v>
       </c>
       <c r="O12" t="s">
-        <v>95</v>
+        <v>131</v>
       </c>
       <c r="P12">
         <v>-1</v>
       </c>
-      <c r="Q12">
-        <v>-1</v>
+      <c r="Q12" s="14">
+        <v>0.23998437481884416</v>
       </c>
       <c r="R12">
-        <v>-1</v>
+        <v>25</v>
       </c>
       <c r="S12">
-        <v>-1</v>
+        <v>2.4613297730699988</v>
       </c>
       <c r="T12">
-        <v>-1</v>
+        <v>0.97499771490187936</v>
       </c>
       <c r="U12">
-        <v>73.099415204678365</v>
+        <v>98.830409356725141</v>
       </c>
       <c r="V12">
-        <v>94.736842105263165</v>
+        <v>100</v>
       </c>
       <c r="W12" t="s">
-        <v>96</v>
+        <v>132</v>
       </c>
       <c r="X12" t="s">
-        <v>78</v>
+        <v>133</v>
       </c>
       <c r="Y12" s="12">
-        <v>11</v>
-      </c>
-      <c r="Z12">
-        <v>1</v>
-      </c>
-      <c r="AA12">
-        <v>2</v>
-      </c>
-      <c r="AB12" s="8">
+        <v>109</v>
+      </c>
+      <c r="Z12" s="5">
+        <v>1</v>
+      </c>
+      <c r="AA12" s="5">
+        <v>2</v>
+      </c>
+      <c r="AB12" s="13">
         <f>AVERAGE(U12:V12)</f>
-        <v>83.918128654970758</v>
-      </c>
-      <c r="AC12">
+        <v>99.415204678362571</v>
+      </c>
+      <c r="AC12" s="13">
+        <f>_xlfn.STDEV.S(U12:V12)</f>
+        <v>0.82702547507198876</v>
+      </c>
+      <c r="AD12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>16</v>
       </c>
@@ -2924,8 +3022,12 @@
         <f>AVERAGE(U13:V13)</f>
         <v>57.894736842105267</v>
       </c>
+      <c r="AC13" s="8">
+        <f>_xlfn.STDEV.S(U13:V13)</f>
+        <v>14.88645855129573</v>
+      </c>
     </row>
-    <row r="14" spans="1:29" s="8" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8">
         <v>27</v>
       </c>
@@ -3011,8 +3113,12 @@
         <f>AVERAGE(U14:V14)</f>
         <v>70.760233918128662</v>
       </c>
+      <c r="AC14" s="8">
+        <f>_xlfn.STDEV.S(U14:V14)</f>
+        <v>10.751331175935738</v>
+      </c>
     </row>
-    <row r="15" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>22</v>
       </c>
@@ -3098,16 +3204,20 @@
         <f>AVERAGE(U15:V15)</f>
         <v>65.497076023391827</v>
       </c>
+      <c r="AC15" s="8">
+        <f>_xlfn.STDEV.S(U15:V15)</f>
+        <v>4.135127375359934</v>
+      </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C16">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -3143,7 +3253,7 @@
         <v>1</v>
       </c>
       <c r="O16" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="P16">
         <v>-1</v>
@@ -3161,19 +3271,19 @@
         <v>-1</v>
       </c>
       <c r="U16">
-        <v>77.192982456140356</v>
+        <v>83.040935672514621</v>
       </c>
       <c r="V16">
-        <v>73.684210526315795</v>
+        <v>89.473684210526315</v>
       </c>
       <c r="W16" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="X16" t="s">
         <v>78</v>
       </c>
       <c r="Y16" s="12">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="Z16">
         <v>1</v>
@@ -3181,15 +3291,19 @@
       <c r="AA16">
         <v>2</v>
       </c>
-      <c r="AB16" s="8">
+      <c r="AB16" s="13">
         <f>AVERAGE(U16:V16)</f>
-        <v>75.438596491228083</v>
-      </c>
-      <c r="AC16">
+        <v>86.257309941520475</v>
+      </c>
+      <c r="AC16" s="13">
+        <f>_xlfn.STDEV.S(U16:V16)</f>
+        <v>4.5486401128959182</v>
+      </c>
+      <c r="AD16">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>26</v>
       </c>
@@ -3275,8 +3389,12 @@
         <f>AVERAGE(U17:V17)</f>
         <v>58.187134502923982</v>
       </c>
+      <c r="AC17" s="8">
+        <f>_xlfn.STDEV.S(U17:V17)</f>
+        <v>7.8567420131838483</v>
+      </c>
     </row>
-    <row r="18" spans="1:29" s="8" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:30" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="10">
         <v>85</v>
       </c>
@@ -3362,8 +3480,12 @@
         <f>AVERAGE(U18:V18)</f>
         <v>77.192982454999992</v>
       </c>
+      <c r="AC18" s="8">
+        <f>_xlfn.STDEV.S(U18:V18)</f>
+        <v>12.405382126700216</v>
+      </c>
     </row>
-    <row r="19" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
         <v>197</v>
       </c>
@@ -3449,8 +3571,12 @@
         <f>AVERAGE(U19:V19)</f>
         <v>79.824561404999997</v>
       </c>
+      <c r="AC19" s="8">
+        <f>_xlfn.STDEV.S(U19:V19)</f>
+        <v>8.6837674851544957</v>
+      </c>
     </row>
-    <row r="20" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5">
         <v>337</v>
       </c>
@@ -3536,8 +3662,12 @@
         <f>AVERAGE(U20:V20)</f>
         <v>79.824561404999997</v>
       </c>
+      <c r="AC20" s="8">
+        <f>_xlfn.STDEV.S(U20:V20)</f>
+        <v>8.6837674851544957</v>
+      </c>
     </row>
-    <row r="21" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5">
         <v>617</v>
       </c>
@@ -3623,8 +3753,12 @@
         <f>AVERAGE(U21:V21)</f>
         <v>79.824561404999997</v>
       </c>
+      <c r="AC21" s="8">
+        <f>_xlfn.STDEV.S(U21:V21)</f>
+        <v>8.6837674851544957</v>
+      </c>
     </row>
-    <row r="22" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>397</v>
       </c>
@@ -3710,8 +3844,12 @@
         <f>AVERAGE(U22:V22)</f>
         <v>79.532163742690059</v>
       </c>
+      <c r="AC22" s="8">
+        <f>_xlfn.STDEV.S(U22:V22)</f>
+        <v>8.2702547507198485</v>
+      </c>
     </row>
-    <row r="23" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>226</v>
       </c>
@@ -3797,8 +3935,12 @@
         <f>AVERAGE(U23:V23)</f>
         <v>79.239766081871352</v>
       </c>
+      <c r="AC23" s="8">
+        <f>_xlfn.STDEV.S(U23:V23)</f>
+        <v>14.472945813759667</v>
+      </c>
     </row>
-    <row r="24" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>30</v>
       </c>
@@ -3884,8 +4026,12 @@
         <f>AVERAGE(U24:V24)</f>
         <v>58.771929824561411</v>
       </c>
+      <c r="AC24" s="8">
+        <f>_xlfn.STDEV.S(U24:V24)</f>
+        <v>16.126996763903719</v>
+      </c>
     </row>
-    <row r="25" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>198</v>
       </c>
@@ -3971,8 +4117,12 @@
         <f>AVERAGE(U25:V25)</f>
         <v>69.298245614035096</v>
       </c>
+      <c r="AC25" s="8">
+        <f>_xlfn.STDEV.S(U25:V25)</f>
+        <v>1.2405382126079731</v>
+      </c>
     </row>
-    <row r="26" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>422</v>
       </c>
@@ -4058,8 +4208,12 @@
         <f>AVERAGE(U26:V26)</f>
         <v>66.959064327485379</v>
       </c>
+      <c r="AC26" s="8">
+        <f>_xlfn.STDEV.S(U26:V26)</f>
+        <v>5.3756655879678918</v>
+      </c>
     </row>
-    <row r="27" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>450</v>
       </c>
@@ -4145,8 +4299,12 @@
         <f>AVERAGE(U27:V27)</f>
         <v>69.883040935672511</v>
       </c>
+      <c r="AC27" s="8">
+        <f>_xlfn.STDEV.S(U27:V27)</f>
+        <v>2.0675636876799519</v>
+      </c>
     </row>
-    <row r="28" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>116</v>
       </c>
@@ -4232,8 +4390,12 @@
         <f>AVERAGE(U28:V28)</f>
         <v>88.596491228070178</v>
       </c>
+      <c r="AC28" s="8">
+        <f>_xlfn.STDEV.S(U28:V28)</f>
+        <v>16.126996763903719</v>
+      </c>
     </row>
-    <row r="29" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>173</v>
       </c>
@@ -4319,8 +4481,12 @@
         <f>AVERAGE(U29:V29)</f>
         <v>85.672514619883046</v>
       </c>
+      <c r="AC29" s="8">
+        <f>_xlfn.STDEV.S(U29:V29)</f>
+        <v>12.818894863615721</v>
+      </c>
     </row>
-    <row r="30" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>145</v>
       </c>
@@ -4406,25 +4572,29 @@
         <f>AVERAGE(U30:V30)</f>
         <v>85.964912280701753</v>
       </c>
+      <c r="AC30" s="8">
+        <f>_xlfn.STDEV.S(U30:V30)</f>
+        <v>12.405382126079829</v>
+      </c>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>510</v>
+        <v>207</v>
       </c>
       <c r="B31">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D31">
         <v>2</v>
       </c>
       <c r="E31">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="F31">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="G31">
         <v>-1</v>
@@ -4451,37 +4621,37 @@
         <v>1</v>
       </c>
       <c r="O31" t="s">
-        <v>403</v>
+        <v>56</v>
       </c>
       <c r="P31">
-        <v>575</v>
-      </c>
-      <c r="Q31">
-        <v>4.9107899495603409E-2</v>
+        <v>423</v>
+      </c>
+      <c r="Q31" s="14">
+        <v>4.9093983780002071E-2</v>
       </c>
       <c r="R31">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="S31">
-        <v>14.013008146414252</v>
+        <v>34.009311832803391</v>
       </c>
       <c r="T31">
-        <v>0.97633724382374631</v>
+        <v>0.96800211479470355</v>
       </c>
       <c r="U31">
-        <v>82.456140350877192</v>
+        <v>88.888888888888886</v>
       </c>
       <c r="V31">
-        <v>94.736842105263165</v>
+        <v>100</v>
       </c>
       <c r="W31" t="s">
-        <v>404</v>
+        <v>57</v>
       </c>
       <c r="X31" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="Y31" s="12">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="Z31" s="5">
         <v>1</v>
@@ -4489,15 +4659,19 @@
       <c r="AA31" s="5">
         <v>2</v>
       </c>
-      <c r="AB31" s="8">
+      <c r="AB31" s="13">
         <f>AVERAGE(U31:V31)</f>
-        <v>88.596491228070178</v>
-      </c>
-      <c r="AC31">
+        <v>94.444444444444443</v>
+      </c>
+      <c r="AC31" s="13">
+        <f>_xlfn.STDEV.S(U31:V31)</f>
+        <v>7.8567420131838634</v>
+      </c>
+      <c r="AD31">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>253</v>
       </c>
@@ -4583,8 +4757,12 @@
         <f>AVERAGE(U32:V32)</f>
         <v>86.257309941520475</v>
       </c>
+      <c r="AC32" s="8">
+        <f>_xlfn.STDEV.S(U32:V32)</f>
+        <v>4.5486401128959182</v>
+      </c>
     </row>
-    <row r="33" spans="1:28" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>147</v>
       </c>
@@ -4670,8 +4848,12 @@
         <f>AVERAGE(U33:V33)</f>
         <v>61.403508771929836</v>
       </c>
+      <c r="AC33" s="8">
+        <f>_xlfn.STDEV.S(U33:V33)</f>
+        <v>27.291840677375507</v>
+      </c>
     </row>
-    <row r="34" spans="1:28" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>30</v>
       </c>
@@ -4757,8 +4939,12 @@
         <f>AVERAGE(U34:V34)</f>
         <v>58.771929824561411</v>
       </c>
+      <c r="AC34" s="8">
+        <f>_xlfn.STDEV.S(U34:V34)</f>
+        <v>16.126996763903719</v>
+      </c>
     </row>
-    <row r="35" spans="1:28" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>87</v>
       </c>
@@ -4844,8 +5030,12 @@
         <f>AVERAGE(U35:V35)</f>
         <v>63.742690058479539</v>
       </c>
+      <c r="AC35" s="8">
+        <f>_xlfn.STDEV.S(U35:V35)</f>
+        <v>23.156713302015579</v>
+      </c>
     </row>
-    <row r="36" spans="1:28" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>284</v>
       </c>
@@ -4931,8 +5121,12 @@
         <f>AVERAGE(U36:V36)</f>
         <v>65.789473684210535</v>
       </c>
+      <c r="AC36" s="8">
+        <f>_xlfn.STDEV.S(U36:V36)</f>
+        <v>26.051302464767549</v>
+      </c>
     </row>
-    <row r="37" spans="1:28" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>590</v>
       </c>
@@ -5018,8 +5212,12 @@
         <f>AVERAGE(U37:V37)</f>
         <v>66.666666666666686</v>
       </c>
+      <c r="AC37" s="8">
+        <f>_xlfn.STDEV.S(U37:V37)</f>
+        <v>19.848611401727588</v>
+      </c>
     </row>
-    <row r="38" spans="1:28" s="8" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:29" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="8">
         <v>711</v>
       </c>
@@ -5105,8 +5303,12 @@
         <f>AVERAGE(U38:V38)</f>
         <v>80.701754385964918</v>
       </c>
+      <c r="AC38" s="8">
+        <f>_xlfn.STDEV.S(U38:V38)</f>
+        <v>17.367534976511688</v>
+      </c>
     </row>
-    <row r="39" spans="1:28" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>95</v>
       </c>
@@ -5192,8 +5394,12 @@
         <f>AVERAGE(U39:V39)</f>
         <v>93.567251461988306</v>
       </c>
+      <c r="AC39" s="8">
+        <f>_xlfn.STDEV.S(U39:V39)</f>
+        <v>1.6540509501439775</v>
+      </c>
     </row>
-    <row r="40" spans="1:28" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>179</v>
       </c>
@@ -5279,8 +5485,12 @@
         <f>AVERAGE(U40:V40)</f>
         <v>85.672514619883032</v>
       </c>
+      <c r="AC40" s="8">
+        <f>_xlfn.STDEV.S(U40:V40)</f>
+        <v>9.5107929633278303</v>
+      </c>
     </row>
-    <row r="41" spans="1:28" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>123</v>
       </c>
@@ -5366,8 +5576,12 @@
         <f>AVERAGE(U41:V41)</f>
         <v>88.011695906432749</v>
       </c>
+      <c r="AC41" s="8">
+        <f>_xlfn.STDEV.S(U41:V41)</f>
+        <v>5.3756655879678972</v>
+      </c>
     </row>
-    <row r="42" spans="1:28" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>291</v>
       </c>
@@ -5453,8 +5667,12 @@
         <f>AVERAGE(U42:V42)</f>
         <v>85.087719298245617</v>
       </c>
+      <c r="AC42" s="8">
+        <f>_xlfn.STDEV.S(U42:V42)</f>
+        <v>8.6837674882558531</v>
+      </c>
     </row>
-    <row r="43" spans="1:28" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>124</v>
       </c>
@@ -5540,8 +5758,12 @@
         <f>AVERAGE(U43:V43)</f>
         <v>66.081871345029242</v>
       </c>
+      <c r="AC43" s="8">
+        <f>_xlfn.STDEV.S(U43:V43)</f>
+        <v>4.1351273753599189</v>
+      </c>
     </row>
-    <row r="44" spans="1:28" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>516</v>
       </c>
@@ -5627,8 +5849,12 @@
         <f>AVERAGE(U44:V44)</f>
         <v>60.818713450292407</v>
       </c>
+      <c r="AC44" s="8">
+        <f>_xlfn.STDEV.S(U44:V44)</f>
+        <v>11.578356651007779</v>
+      </c>
     </row>
-    <row r="45" spans="1:28" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>40</v>
       </c>
@@ -5714,8 +5940,12 @@
         <f>AVERAGE(U45:V45)</f>
         <v>69.298245614035096</v>
       </c>
+      <c r="AC45" s="8">
+        <f>_xlfn.STDEV.S(U45:V45)</f>
+        <v>1.2405382126079731</v>
+      </c>
     </row>
-    <row r="46" spans="1:28" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>656</v>
       </c>
@@ -5801,8 +6031,12 @@
         <f>AVERAGE(U46:V46)</f>
         <v>69.298245614035096</v>
       </c>
+      <c r="AC46" s="8">
+        <f>_xlfn.STDEV.S(U46:V46)</f>
+        <v>1.2405382126079731</v>
+      </c>
     </row>
-    <row r="47" spans="1:28" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>544</v>
       </c>
@@ -5888,8 +6122,12 @@
         <f>AVERAGE(U47:V47)</f>
         <v>69.590643274853804</v>
       </c>
+      <c r="AC47" s="8">
+        <f>_xlfn.STDEV.S(U47:V47)</f>
+        <v>1.6540509501439575</v>
+      </c>
     </row>
-    <row r="48" spans="1:28" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>235</v>
       </c>
@@ -5975,28 +6213,32 @@
         <f>AVERAGE(U48:V48)</f>
         <v>94.152046783625735</v>
       </c>
+      <c r="AC48" s="8">
+        <f>_xlfn.STDEV.S(U48:V48)</f>
+        <v>8.2702547507198574</v>
+      </c>
     </row>
-    <row r="49" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>207</v>
+        <v>988</v>
       </c>
       <c r="B49">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C49">
         <v>2</v>
       </c>
       <c r="D49">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E49">
-        <v>2000</v>
+        <v>5000</v>
       </c>
       <c r="F49">
-        <v>0.4</v>
+        <v>400</v>
       </c>
       <c r="G49">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="H49" t="s">
         <v>0</v>
@@ -6020,37 +6262,37 @@
         <v>1</v>
       </c>
       <c r="O49" t="s">
-        <v>56</v>
+        <v>164</v>
       </c>
       <c r="P49">
-        <v>423</v>
-      </c>
-      <c r="Q49">
-        <v>4.9093983780002071E-2</v>
+        <v>-1</v>
+      </c>
+      <c r="Q49" s="14">
+        <v>0.10657300027280581</v>
       </c>
       <c r="R49">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="S49">
-        <v>34.009311832803391</v>
+        <v>68.658549414427569</v>
       </c>
       <c r="T49">
-        <v>0.96800211479470355</v>
+        <v>0.96400093014269161</v>
       </c>
       <c r="U49">
-        <v>88.888888888888886</v>
+        <v>99.415204678362571</v>
       </c>
       <c r="V49">
         <v>100</v>
       </c>
       <c r="W49" t="s">
-        <v>57</v>
+        <v>165</v>
       </c>
       <c r="X49" t="s">
-        <v>31</v>
+        <v>166</v>
       </c>
       <c r="Y49" s="12">
-        <v>48</v>
+        <v>127</v>
       </c>
       <c r="Z49" s="5">
         <v>1</v>
@@ -6058,15 +6300,19 @@
       <c r="AA49" s="5">
         <v>2</v>
       </c>
-      <c r="AB49" s="8">
+      <c r="AB49" s="13">
         <f>AVERAGE(U49:V49)</f>
-        <v>94.444444444444443</v>
-      </c>
-      <c r="AC49">
+        <v>99.707602339181278</v>
+      </c>
+      <c r="AC49" s="13">
+        <f>_xlfn.STDEV.S(U49:V49)</f>
+        <v>0.41351273753599438</v>
+      </c>
+      <c r="AD49">
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>321</v>
       </c>
@@ -6152,8 +6398,12 @@
         <f>AVERAGE(U50:V50)</f>
         <v>91.520467836257311</v>
       </c>
+      <c r="AC50" s="8">
+        <f>_xlfn.STDEV.S(U50:V50)</f>
+        <v>4.548640112895928</v>
+      </c>
     </row>
-    <row r="51" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>431</v>
       </c>
@@ -6239,8 +6489,12 @@
         <f>AVERAGE(U51:V51)</f>
         <v>91.520467836257311</v>
       </c>
+      <c r="AC51" s="8">
+        <f>_xlfn.STDEV.S(U51:V51)</f>
+        <v>4.548640112895928</v>
+      </c>
     </row>
-    <row r="52" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>95</v>
       </c>
@@ -6326,8 +6580,12 @@
         <f>AVERAGE(U52:V52)</f>
         <v>93.567251461988306</v>
       </c>
+      <c r="AC52" s="8">
+        <f>_xlfn.STDEV.S(U52:V52)</f>
+        <v>1.6540509501439775</v>
+      </c>
     </row>
-    <row r="53" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>68</v>
       </c>
@@ -6413,8 +6671,12 @@
         <f>AVERAGE(U53:V53)</f>
         <v>61.403508771929829</v>
       </c>
+      <c r="AC53" s="8">
+        <f>_xlfn.STDEV.S(U53:V53)</f>
+        <v>19.848611401727659</v>
+      </c>
     </row>
-    <row r="54" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>516</v>
       </c>
@@ -6500,8 +6762,12 @@
         <f>AVERAGE(U54:V54)</f>
         <v>60.818713450292407</v>
       </c>
+      <c r="AC54" s="8">
+        <f>_xlfn.STDEV.S(U54:V54)</f>
+        <v>11.578356651007779</v>
+      </c>
     </row>
-    <row r="55" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>460</v>
       </c>
@@ -6587,8 +6853,12 @@
         <f>AVERAGE(U55:V55)</f>
         <v>62.280701754385973</v>
       </c>
+      <c r="AC55" s="8">
+        <f>_xlfn.STDEV.S(U55:V55)</f>
+        <v>13.64592033868772</v>
+      </c>
     </row>
-    <row r="56" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>346</v>
       </c>
@@ -6674,8 +6944,12 @@
         <f>AVERAGE(U56:V56)</f>
         <v>63.742690058479539</v>
       </c>
+      <c r="AC56" s="8">
+        <f>_xlfn.STDEV.S(U56:V56)</f>
+        <v>15.713484026367695</v>
+      </c>
     </row>
-    <row r="57" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>232</v>
       </c>
@@ -6761,8 +7035,12 @@
         <f>AVERAGE(U57:V57)</f>
         <v>65.789473684210535</v>
       </c>
+      <c r="AC57" s="8">
+        <f>_xlfn.STDEV.S(U57:V57)</f>
+        <v>18.608073189119693</v>
+      </c>
     </row>
-    <row r="58" spans="1:29" s="8" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:30" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="8">
         <v>575</v>
       </c>
@@ -6848,8 +7126,12 @@
         <f>AVERAGE(U58:V58)</f>
         <v>85.087719298245617</v>
       </c>
+      <c r="AC58" s="8">
+        <f>_xlfn.STDEV.S(U58:V58)</f>
+        <v>8.6837674882558531</v>
+      </c>
     </row>
-    <row r="59" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>635</v>
       </c>
@@ -6935,8 +7217,12 @@
         <f>AVERAGE(U59:V59)</f>
         <v>84.795321637426895</v>
       </c>
+      <c r="AC59" s="8">
+        <f>_xlfn.STDEV.S(U59:V59)</f>
+        <v>8.2702547507198574</v>
+      </c>
     </row>
-    <row r="60" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>691</v>
       </c>
@@ -7022,8 +7308,12 @@
         <f>AVERAGE(U60:V60)</f>
         <v>87.134502923976612</v>
       </c>
+      <c r="AC60" s="8">
+        <f>_xlfn.STDEV.S(U60:V60)</f>
+        <v>4.1351273753599243</v>
+      </c>
     </row>
-    <row r="61" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>75</v>
       </c>
@@ -7109,8 +7399,12 @@
         <f>AVERAGE(U61:V61)</f>
         <v>86.549707602339183</v>
       </c>
+      <c r="AC61" s="8">
+        <f>_xlfn.STDEV.S(U61:V61)</f>
+        <v>3.308101900287935</v>
+      </c>
     </row>
-    <row r="62" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>299</v>
       </c>
@@ -7196,8 +7490,12 @@
         <f>AVERAGE(U62:V62)</f>
         <v>89.181286549707607</v>
       </c>
+      <c r="AC62" s="8">
+        <f>_xlfn.STDEV.S(U62:V62)</f>
+        <v>0.41351273753599438</v>
+      </c>
     </row>
-    <row r="63" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>520</v>
       </c>
@@ -7283,8 +7581,12 @@
         <f>AVERAGE(U63:V63)</f>
         <v>66.959064327485379</v>
       </c>
+      <c r="AC63" s="8">
+        <f>_xlfn.STDEV.S(U63:V63)</f>
+        <v>2.0675636876799719</v>
+      </c>
     </row>
-    <row r="64" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>632</v>
       </c>
@@ -7370,8 +7672,12 @@
         <f>AVERAGE(U64:V64)</f>
         <v>64.619883040935676</v>
       </c>
+      <c r="AC64" s="8">
+        <f>_xlfn.STDEV.S(U64:V64)</f>
+        <v>2.0675636876799568</v>
+      </c>
     </row>
-    <row r="65" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>660</v>
       </c>
@@ -7457,8 +7763,12 @@
         <f>AVERAGE(U65:V65)</f>
         <v>61.988304093567258</v>
       </c>
+      <c r="AC65" s="8">
+        <f>_xlfn.STDEV.S(U65:V65)</f>
+        <v>5.7891783255038911</v>
+      </c>
     </row>
-    <row r="66" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>716</v>
       </c>
@@ -7544,8 +7854,12 @@
         <f>AVERAGE(U66:V66)</f>
         <v>59.356725146198841</v>
       </c>
+      <c r="AC66" s="8">
+        <f>_xlfn.STDEV.S(U66:V66)</f>
+        <v>9.5107929633277983</v>
+      </c>
     </row>
-    <row r="67" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>604</v>
       </c>
@@ -7631,25 +7945,29 @@
         <f>AVERAGE(U67:V67)</f>
         <v>67.543859649122822</v>
       </c>
+      <c r="AC67" s="8">
+        <f>_xlfn.STDEV.S(U67:V67)</f>
+        <v>1.2405382126079834</v>
+      </c>
     </row>
-    <row r="68" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>521</v>
+        <v>20</v>
       </c>
       <c r="B68">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C68">
         <v>3</v>
       </c>
       <c r="D68">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E68">
-        <v>3000</v>
+        <v>-1</v>
       </c>
       <c r="F68">
-        <v>0.6</v>
+        <v>-1</v>
       </c>
       <c r="G68">
         <v>-1</v>
@@ -7676,53 +7994,57 @@
         <v>1</v>
       </c>
       <c r="O68" t="s">
-        <v>61</v>
+        <v>95</v>
       </c>
       <c r="P68">
-        <v>742</v>
+        <v>-1</v>
       </c>
       <c r="Q68">
-        <v>3.6938157400291959E-2</v>
+        <v>-1</v>
       </c>
       <c r="R68">
-        <v>20</v>
+        <v>-1</v>
       </c>
       <c r="S68">
-        <v>4.3351526166221896</v>
+        <v>-1</v>
       </c>
       <c r="T68">
-        <v>0.99222984228646471</v>
+        <v>-1</v>
       </c>
       <c r="U68">
-        <v>87.134502923976612</v>
+        <v>73.099415204678365</v>
       </c>
       <c r="V68">
-        <v>100</v>
+        <v>94.736842105263165</v>
       </c>
       <c r="W68" t="s">
-        <v>62</v>
+        <v>96</v>
       </c>
       <c r="X68" t="s">
-        <v>50</v>
+        <v>78</v>
       </c>
       <c r="Y68" s="12">
-        <v>67</v>
-      </c>
-      <c r="Z68" s="5">
-        <v>1</v>
-      </c>
-      <c r="AA68" s="5">
-        <v>2</v>
-      </c>
-      <c r="AB68" s="8">
+        <v>11</v>
+      </c>
+      <c r="Z68">
+        <v>1</v>
+      </c>
+      <c r="AA68">
+        <v>2</v>
+      </c>
+      <c r="AB68" s="13">
         <f>AVERAGE(U68:V68)</f>
-        <v>93.567251461988306</v>
-      </c>
-      <c r="AC68">
+        <v>83.918128654970758</v>
+      </c>
+      <c r="AC68" s="13">
+        <f>_xlfn.STDEV.S(U68:V68)</f>
+        <v>15.299971288831749</v>
+      </c>
+      <c r="AD68">
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>551</v>
       </c>
@@ -7808,8 +8130,12 @@
         <f>AVERAGE(U69:V69)</f>
         <v>88.596491228070178</v>
       </c>
+      <c r="AC69" s="8">
+        <f>_xlfn.STDEV.S(U69:V69)</f>
+        <v>8.6837674882558531</v>
+      </c>
     </row>
-    <row r="70" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>325</v>
       </c>
@@ -7895,8 +8221,12 @@
         <f>AVERAGE(U70:V70)</f>
         <v>89.766081871345023</v>
       </c>
+      <c r="AC70" s="8">
+        <f>_xlfn.STDEV.S(U70:V70)</f>
+        <v>7.0297165381118853</v>
+      </c>
     </row>
-    <row r="71" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>439</v>
       </c>
@@ -7982,8 +8312,12 @@
         <f>AVERAGE(U71:V71)</f>
         <v>89.766081871345023</v>
       </c>
+      <c r="AC71" s="8">
+        <f>_xlfn.STDEV.S(U71:V71)</f>
+        <v>7.0297165381118853</v>
+      </c>
     </row>
-    <row r="72" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>239</v>
       </c>
@@ -8069,8 +8403,12 @@
         <f>AVERAGE(U72:V72)</f>
         <v>90.935672514619881</v>
       </c>
+      <c r="AC72" s="8">
+        <f>_xlfn.STDEV.S(U72:V72)</f>
+        <v>5.3756655879679069</v>
+      </c>
     </row>
-    <row r="73" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>492</v>
       </c>
@@ -8156,8 +8494,12 @@
         <f>AVERAGE(U73:V73)</f>
         <v>55.555555555555557</v>
       </c>
+      <c r="AC73" s="8">
+        <f>_xlfn.STDEV.S(U73:V73)</f>
+        <v>19.021585926655693</v>
+      </c>
     </row>
-    <row r="74" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>464</v>
       </c>
@@ -8243,8 +8585,12 @@
         <f>AVERAGE(U74:V74)</f>
         <v>58.479532163742697</v>
       </c>
+      <c r="AC74" s="8">
+        <f>_xlfn.STDEV.S(U74:V74)</f>
+        <v>15.713484026367695</v>
+      </c>
     </row>
-    <row r="75" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>716</v>
       </c>
@@ -8330,8 +8676,12 @@
         <f>AVERAGE(U75:V75)</f>
         <v>59.356725146198841</v>
       </c>
+      <c r="AC75" s="8">
+        <f>_xlfn.STDEV.S(U75:V75)</f>
+        <v>9.5107929633277983</v>
+      </c>
     </row>
-    <row r="76" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>156</v>
       </c>
@@ -8417,8 +8767,12 @@
         <f>AVERAGE(U76:V76)</f>
         <v>60.818713450292407</v>
       </c>
+      <c r="AC76" s="8">
+        <f>_xlfn.STDEV.S(U76:V76)</f>
+        <v>11.578356651007779</v>
+      </c>
     </row>
-    <row r="77" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>216</v>
       </c>
@@ -8504,8 +8858,12 @@
         <f>AVERAGE(U77:V77)</f>
         <v>64.61988304093569</v>
       </c>
+      <c r="AC77" s="8">
+        <f>_xlfn.STDEV.S(U77:V77)</f>
+        <v>16.954022238975647</v>
+      </c>
     </row>
-    <row r="78" spans="1:29" s="8" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:30" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="8">
         <v>389</v>
       </c>
@@ -8591,8 +8949,12 @@
         <f>AVERAGE(U78:V78)</f>
         <v>78.654970760233923</v>
       </c>
+      <c r="AC78" s="8">
+        <f>_xlfn.STDEV.S(U78:V78)</f>
+        <v>7.0297165381118747</v>
+      </c>
     </row>
-    <row r="79" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>447</v>
       </c>
@@ -8678,8 +9040,12 @@
         <f>AVERAGE(U79:V79)</f>
         <v>72.807017543859658</v>
       </c>
+      <c r="AC79" s="8">
+        <f>_xlfn.STDEV.S(U79:V79)</f>
+        <v>13.645920338687787</v>
+      </c>
     </row>
-    <row r="80" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>307</v>
       </c>
@@ -8765,8 +9131,12 @@
         <f>AVERAGE(U80:V80)</f>
         <v>75.146198830409361</v>
       </c>
+      <c r="AC80" s="8">
+        <f>_xlfn.STDEV.S(U80:V80)</f>
+        <v>9.5107929633278214</v>
+      </c>
     </row>
-    <row r="81" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>167</v>
       </c>
@@ -8852,8 +9222,12 @@
         <f>AVERAGE(U81:V81)</f>
         <v>80.116959064327489</v>
       </c>
+      <c r="AC81" s="8">
+        <f>_xlfn.STDEV.S(U81:V81)</f>
+        <v>1.6540509501439675</v>
+      </c>
     </row>
-    <row r="82" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>616</v>
       </c>
@@ -8939,8 +9313,12 @@
         <f>AVERAGE(U82:V82)</f>
         <v>80.116959064327489</v>
       </c>
+      <c r="AC82" s="8">
+        <f>_xlfn.STDEV.S(U82:V82)</f>
+        <v>1.6540509501439675</v>
+      </c>
     </row>
-    <row r="83" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>583</v>
       </c>
@@ -9026,8 +9404,12 @@
         <f>AVERAGE(U83:V83)</f>
         <v>82.456140350877192</v>
       </c>
+      <c r="AC83" s="8">
+        <f>_xlfn.STDEV.S(U83:V83)</f>
+        <v>24.810764252159547</v>
+      </c>
     </row>
-    <row r="84" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>362</v>
       </c>
@@ -9113,8 +9495,12 @@
         <f>AVERAGE(U84:V84)</f>
         <v>72.222222222222229</v>
       </c>
+      <c r="AC84" s="8">
+        <f>_xlfn.STDEV.S(U84:V84)</f>
+        <v>9.5107929633278303</v>
+      </c>
     </row>
-    <row r="85" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>638</v>
       </c>
@@ -9200,8 +9586,12 @@
         <f>AVERAGE(U85:V85)</f>
         <v>67.251461988304101</v>
       </c>
+      <c r="AC85" s="8">
+        <f>_xlfn.STDEV.S(U85:V85)</f>
+        <v>1.6540509501439775</v>
+      </c>
     </row>
-    <row r="86" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>667</v>
       </c>
@@ -9287,8 +9677,12 @@
         <f>AVERAGE(U86:V86)</f>
         <v>75.146198830409361</v>
       </c>
+      <c r="AC86" s="8">
+        <f>_xlfn.STDEV.S(U86:V86)</f>
+        <v>12.818894863615792</v>
+      </c>
     </row>
-    <row r="87" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>192</v>
       </c>
@@ -9374,8 +9768,12 @@
         <f>AVERAGE(U87:V87)</f>
         <v>67.543859649122822</v>
       </c>
+      <c r="AC87" s="8">
+        <f>_xlfn.STDEV.S(U87:V87)</f>
+        <v>1.2405382126079834</v>
+      </c>
     </row>
-    <row r="88" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>583</v>
       </c>
@@ -9461,8 +9859,12 @@
         <f>AVERAGE(U88:V88)</f>
         <v>82.456140350877192</v>
       </c>
+      <c r="AC88" s="8">
+        <f>_xlfn.STDEV.S(U88:V88)</f>
+        <v>24.810764252159547</v>
+      </c>
     </row>
-    <row r="89" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>722</v>
       </c>
@@ -9548,25 +9950,29 @@
         <f>AVERAGE(U89:V89)</f>
         <v>82.163742690058484</v>
       </c>
+      <c r="AC89" s="8">
+        <f>_xlfn.STDEV.S(U89:V89)</f>
+        <v>17.781047714047642</v>
+      </c>
     </row>
-    <row r="90" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A90">
-        <v>224</v>
+        <v>521</v>
       </c>
       <c r="B90">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C90">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D90">
         <v>2</v>
       </c>
       <c r="E90">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="F90">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="G90">
         <v>-1</v>
@@ -9593,37 +9999,37 @@
         <v>1</v>
       </c>
       <c r="O90" t="s">
-        <v>313</v>
+        <v>61</v>
       </c>
       <c r="P90">
-        <v>1080</v>
-      </c>
-      <c r="Q90">
-        <v>3.8844740950470136E-2</v>
+        <v>742</v>
+      </c>
+      <c r="Q90" s="14">
+        <v>3.6938157400291959E-2</v>
       </c>
       <c r="R90">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="S90">
-        <v>19.313113661046593</v>
+        <v>4.3351526166221896</v>
       </c>
       <c r="T90">
-        <v>0.979917810676321</v>
+        <v>0.99222984228646471</v>
       </c>
       <c r="U90">
-        <v>77.777777777777771</v>
+        <v>87.134502923976612</v>
       </c>
       <c r="V90">
-        <v>94.736842105263165</v>
+        <v>100</v>
       </c>
       <c r="W90" t="s">
-        <v>314</v>
+        <v>62</v>
       </c>
       <c r="X90" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="Y90" s="12">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="Z90" s="5">
         <v>1</v>
@@ -9631,15 +10037,19 @@
       <c r="AA90" s="5">
         <v>2</v>
       </c>
-      <c r="AB90" s="8">
+      <c r="AB90" s="13">
         <f>AVERAGE(U90:V90)</f>
-        <v>86.257309941520475</v>
-      </c>
-      <c r="AC90">
+        <v>93.567251461988306</v>
+      </c>
+      <c r="AC90" s="13">
+        <f>_xlfn.STDEV.S(U90:V90)</f>
+        <v>9.0972802257918364</v>
+      </c>
+      <c r="AD90">
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>279</v>
       </c>
@@ -9725,8 +10135,12 @@
         <f>AVERAGE(U91:V91)</f>
         <v>84.21052631578948</v>
       </c>
+      <c r="AC91" s="8">
+        <f>_xlfn.STDEV.S(U91:V91)</f>
+        <v>7.4432292756478695</v>
+      </c>
     </row>
-    <row r="92" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>391</v>
       </c>
@@ -9812,8 +10226,12 @@
         <f>AVERAGE(U92:V92)</f>
         <v>84.502923976608187</v>
       </c>
+      <c r="AC92" s="8">
+        <f>_xlfn.STDEV.S(U92:V92)</f>
+        <v>7.0297165381118747</v>
+      </c>
     </row>
-    <row r="93" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>556</v>
       </c>
@@ -9899,8 +10317,12 @@
         <f>AVERAGE(U93:V93)</f>
         <v>55.847953216374279</v>
       </c>
+      <c r="AC93" s="8">
+        <f>_xlfn.STDEV.S(U93:V93)</f>
+        <v>19.435098664191631</v>
+      </c>
     </row>
-    <row r="94" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>554</v>
       </c>
@@ -9986,8 +10408,12 @@
         <f>AVERAGE(U94:V94)</f>
         <v>57.017543859649123</v>
       </c>
+      <c r="AC94" s="8">
+        <f>_xlfn.STDEV.S(U94:V94)</f>
+        <v>21.089149614335632</v>
+      </c>
     </row>
-    <row r="95" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>558</v>
       </c>
@@ -10073,8 +10499,12 @@
         <f>AVERAGE(U95:V95)</f>
         <v>57.602339181286553</v>
       </c>
+      <c r="AC95" s="8">
+        <f>_xlfn.STDEV.S(U95:V95)</f>
+        <v>21.916175089407623</v>
+      </c>
     </row>
-    <row r="96" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>498</v>
       </c>
@@ -10160,8 +10590,12 @@
         <f>AVERAGE(U96:V96)</f>
         <v>58.771929824561411</v>
       </c>
+      <c r="AC96" s="8">
+        <f>_xlfn.STDEV.S(U96:V96)</f>
+        <v>23.570226039551567</v>
+      </c>
     </row>
-    <row r="97" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>302</v>
       </c>
@@ -10247,8 +10681,12 @@
         <f>AVERAGE(U97:V97)</f>
         <v>58.479532163742697</v>
       </c>
+      <c r="AC97" s="8">
+        <f>_xlfn.STDEV.S(U97:V97)</f>
+        <v>15.713484026367695</v>
+      </c>
     </row>
-    <row r="98" spans="1:29" s="8" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:30" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="8">
         <v>1687</v>
       </c>
@@ -10334,8 +10772,12 @@
         <f>AVERAGE(U98:V98)</f>
         <v>84.21052631578948</v>
       </c>
+      <c r="AC98" s="8">
+        <f>_xlfn.STDEV.S(U98:V98)</f>
+        <v>22.329687826943577</v>
+      </c>
     </row>
-    <row r="99" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>2359</v>
       </c>
@@ -10421,8 +10863,12 @@
         <f>AVERAGE(U99:V99)</f>
         <v>86.84210526315789</v>
       </c>
+      <c r="AC99" s="8">
+        <f>_xlfn.STDEV.S(U99:V99)</f>
+        <v>18.608073189119743</v>
+      </c>
     </row>
-    <row r="100" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>3395</v>
       </c>
@@ -10508,8 +10954,12 @@
         <f>AVERAGE(U100:V100)</f>
         <v>92.10526315789474</v>
       </c>
+      <c r="AC100" s="8">
+        <f>_xlfn.STDEV.S(U100:V100)</f>
+        <v>11.164843913471799</v>
+      </c>
     </row>
-    <row r="101" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>3672</v>
       </c>
@@ -10595,8 +11045,12 @@
         <f>AVERAGE(U101:V101)</f>
         <v>86.84210526315789</v>
       </c>
+      <c r="AC101" s="8">
+        <f>_xlfn.STDEV.S(U101:V101)</f>
+        <v>18.608073189119743</v>
+      </c>
     </row>
-    <row r="102" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>3977</v>
       </c>
@@ -10682,8 +11136,12 @@
         <f>AVERAGE(U102:V102)</f>
         <v>97.368421052631589</v>
       </c>
+      <c r="AC102" s="8">
+        <f>_xlfn.STDEV.S(U102:V102)</f>
+        <v>3.7216146378239299</v>
+      </c>
     </row>
-    <row r="103" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>1321</v>
       </c>
@@ -10769,8 +11227,12 @@
         <f>AVERAGE(U103:V103)</f>
         <v>52.631578947368425</v>
       </c>
+      <c r="AC103" s="8">
+        <f>_xlfn.STDEV.S(U103:V103)</f>
+        <v>1.5888218580782548E-14</v>
+      </c>
     </row>
-    <row r="104" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>1065</v>
       </c>
@@ -10856,8 +11318,12 @@
         <f>AVERAGE(U104:V104)</f>
         <v>52.339181286549717</v>
       </c>
+      <c r="AC104" s="8">
+        <f>_xlfn.STDEV.S(U104:V104)</f>
+        <v>7.0297165381118702</v>
+      </c>
     </row>
-    <row r="105" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>1211</v>
       </c>
@@ -10943,8 +11409,12 @@
         <f>AVERAGE(U105:V105)</f>
         <v>47.660818713450297</v>
       </c>
+      <c r="AC105" s="8">
+        <f>_xlfn.STDEV.S(U105:V105)</f>
+        <v>15.299971288831749</v>
+      </c>
     </row>
-    <row r="106" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>1122</v>
       </c>
@@ -11030,8 +11500,12 @@
         <f>AVERAGE(U106:V106)</f>
         <v>48.245614035087726</v>
       </c>
+      <c r="AC106" s="8">
+        <f>_xlfn.STDEV.S(U106:V106)</f>
+        <v>23.570226039551567</v>
+      </c>
     </row>
-    <row r="107" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>1208</v>
       </c>
@@ -11117,8 +11591,12 @@
         <f>AVERAGE(U107:V107)</f>
         <v>46.783625730994153</v>
       </c>
+      <c r="AC107" s="8">
+        <f>_xlfn.STDEV.S(U107:V107)</f>
+        <v>28.945891627519476</v>
+      </c>
     </row>
-    <row r="108" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>3281</v>
       </c>
@@ -11204,8 +11682,12 @@
         <f>AVERAGE(U108:V108)</f>
         <v>99.122807017543863</v>
       </c>
+      <c r="AC108" s="8">
+        <f>_xlfn.STDEV.S(U108:V108)</f>
+        <v>1.2405382126079731</v>
+      </c>
     </row>
-    <row r="109" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>1739</v>
       </c>
@@ -11291,98 +11773,106 @@
         <f>AVERAGE(U109:V109)</f>
         <v>99.415204678362571</v>
       </c>
+      <c r="AC109" s="8">
+        <f>_xlfn.STDEV.S(U109:V109)</f>
+        <v>0.82702547507198876</v>
+      </c>
     </row>
-    <row r="110" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A110">
-        <v>2665</v>
-      </c>
-      <c r="B110">
-        <v>5</v>
-      </c>
-      <c r="C110">
-        <v>1</v>
-      </c>
-      <c r="D110">
-        <v>3</v>
-      </c>
-      <c r="E110">
-        <v>5000</v>
-      </c>
-      <c r="F110">
+    <row r="110" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A110" s="8">
+        <v>1863</v>
+      </c>
+      <c r="B110" s="8">
+        <v>1</v>
+      </c>
+      <c r="C110" s="8">
+        <v>3</v>
+      </c>
+      <c r="D110" s="8">
+        <v>3</v>
+      </c>
+      <c r="E110" s="8">
+        <v>1000</v>
+      </c>
+      <c r="F110" s="8">
         <v>600</v>
       </c>
-      <c r="G110">
-        <v>27.5</v>
-      </c>
-      <c r="H110" t="s">
-        <v>0</v>
-      </c>
-      <c r="I110" t="s">
-        <v>1</v>
-      </c>
-      <c r="J110" t="s">
-        <v>2</v>
-      </c>
-      <c r="K110">
+      <c r="G110" s="8">
+        <v>16.25</v>
+      </c>
+      <c r="H110" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="I110" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="J110" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="K110" s="8">
         <v>0.35</v>
       </c>
-      <c r="L110" t="s">
-        <v>3</v>
-      </c>
-      <c r="M110" t="s">
-        <v>1</v>
-      </c>
-      <c r="N110">
-        <v>1</v>
-      </c>
-      <c r="O110" t="s">
-        <v>131</v>
-      </c>
-      <c r="P110">
-        <v>-1</v>
-      </c>
-      <c r="Q110">
-        <v>0.23998437481884416</v>
-      </c>
-      <c r="R110">
-        <v>25</v>
-      </c>
-      <c r="S110">
-        <v>2.4613297730699988</v>
-      </c>
-      <c r="T110">
-        <v>0.97499771490187936</v>
-      </c>
-      <c r="U110">
-        <v>98.830409356725141</v>
-      </c>
-      <c r="V110">
+      <c r="L110" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="M110" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="N110" s="8">
+        <v>1</v>
+      </c>
+      <c r="O110" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="P110" s="8">
+        <v>-1</v>
+      </c>
+      <c r="Q110" s="13">
+        <v>0.15233663015660426</v>
+      </c>
+      <c r="R110" s="8">
+        <v>16</v>
+      </c>
+      <c r="S110" s="8">
+        <v>3.2968181593662313</v>
+      </c>
+      <c r="T110" s="8">
+        <v>0.99024197092243993</v>
+      </c>
+      <c r="U110" s="8">
         <v>100</v>
       </c>
-      <c r="W110" t="s">
-        <v>132</v>
-      </c>
-      <c r="X110" t="s">
-        <v>133</v>
-      </c>
-      <c r="Y110" s="12">
-        <v>109</v>
-      </c>
-      <c r="Z110" s="5">
-        <v>1</v>
-      </c>
-      <c r="AA110" s="5">
-        <v>2</v>
-      </c>
-      <c r="AB110" s="8">
+      <c r="V110" s="8">
+        <v>100</v>
+      </c>
+      <c r="W110" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="X110" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="Y110" s="8">
+        <v>137</v>
+      </c>
+      <c r="Z110" s="8">
+        <v>1</v>
+      </c>
+      <c r="AA110" s="8">
+        <v>1</v>
+      </c>
+      <c r="AB110" s="13">
         <f>AVERAGE(U110:V110)</f>
-        <v>99.415204678362571</v>
-      </c>
-      <c r="AC110">
+        <v>100</v>
+      </c>
+      <c r="AC110" s="13">
+        <f>_xlfn.STDEV.S(U110:V110)</f>
+        <v>0</v>
+      </c>
+      <c r="AD110" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>2721</v>
       </c>
@@ -11468,8 +11958,12 @@
         <f>AVERAGE(U111:V111)</f>
         <v>99.415204678362571</v>
       </c>
+      <c r="AC111" s="8">
+        <f>_xlfn.STDEV.S(U111:V111)</f>
+        <v>0.82702547507198876</v>
+      </c>
     </row>
-    <row r="112" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>2889</v>
       </c>
@@ -11555,8 +12049,12 @@
         <f>AVERAGE(U112:V112)</f>
         <v>99.415204678362571</v>
       </c>
+      <c r="AC112" s="8">
+        <f>_xlfn.STDEV.S(U112:V112)</f>
+        <v>0.82702547507198876</v>
+      </c>
     </row>
-    <row r="113" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>1154</v>
       </c>
@@ -11642,8 +12140,12 @@
         <f>AVERAGE(U113:V113)</f>
         <v>45.906432748538009</v>
       </c>
+      <c r="AC113" s="8">
+        <f>_xlfn.STDEV.S(U113:V113)</f>
+        <v>42.59181196620726</v>
+      </c>
     </row>
-    <row r="114" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>1236</v>
       </c>
@@ -11729,8 +12231,12 @@
         <f>AVERAGE(U114:V114)</f>
         <v>46.783625730994153</v>
       </c>
+      <c r="AC114" s="8">
+        <f>_xlfn.STDEV.S(U114:V114)</f>
+        <v>36.38912090316736</v>
+      </c>
     </row>
-    <row r="115" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>1180</v>
       </c>
@@ -11816,8 +12322,12 @@
         <f>AVERAGE(U115:V115)</f>
         <v>49.122807017543863</v>
       </c>
+      <c r="AC115" s="8">
+        <f>_xlfn.STDEV.S(U115:V115)</f>
+        <v>32.253993527807424</v>
+      </c>
     </row>
-    <row r="116" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>1347</v>
       </c>
@@ -11903,8 +12413,12 @@
         <f>AVERAGE(U116:V116)</f>
         <v>47.660818713450297</v>
       </c>
+      <c r="AC116" s="8">
+        <f>_xlfn.STDEV.S(U116:V116)</f>
+        <v>30.186429840127474</v>
+      </c>
     </row>
-    <row r="117" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>1208</v>
       </c>
@@ -11990,8 +12504,12 @@
         <f>AVERAGE(U117:V117)</f>
         <v>46.783625730994153</v>
       </c>
+      <c r="AC117" s="8">
+        <f>_xlfn.STDEV.S(U117:V117)</f>
+        <v>28.945891627519476</v>
+      </c>
     </row>
-    <row r="118" spans="1:29" s="8" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:30" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="8">
         <v>1581</v>
       </c>
@@ -12077,8 +12595,12 @@
         <f>AVERAGE(U118:V118)</f>
         <v>97.368421052631589</v>
       </c>
+      <c r="AC118" s="8">
+        <f>_xlfn.STDEV.S(U118:V118)</f>
+        <v>3.7216146378239299</v>
+      </c>
     </row>
-    <row r="119" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>1660</v>
       </c>
@@ -12164,8 +12686,12 @@
         <f>AVERAGE(U119:V119)</f>
         <v>94.73684210526315</v>
       </c>
+      <c r="AC119" s="8">
+        <f>_xlfn.STDEV.S(U119:V119)</f>
+        <v>7.4432292756478695</v>
+      </c>
     </row>
-    <row r="120" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>1940</v>
       </c>
@@ -12251,8 +12777,12 @@
         <f>AVERAGE(U120:V120)</f>
         <v>94.73684210526315</v>
       </c>
+      <c r="AC120" s="8">
+        <f>_xlfn.STDEV.S(U120:V120)</f>
+        <v>7.4432292756478695</v>
+      </c>
     </row>
-    <row r="121" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>2472</v>
       </c>
@@ -12338,8 +12868,12 @@
         <f>AVERAGE(U121:V121)</f>
         <v>94.73684210526315</v>
       </c>
+      <c r="AC121" s="8">
+        <f>_xlfn.STDEV.S(U121:V121)</f>
+        <v>7.4432292756478695</v>
+      </c>
     </row>
-    <row r="122" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>2892</v>
       </c>
@@ -12425,8 +12959,12 @@
         <f>AVERAGE(U122:V122)</f>
         <v>97.368421052631589</v>
       </c>
+      <c r="AC122" s="8">
+        <f>_xlfn.STDEV.S(U122:V122)</f>
+        <v>3.7216146378239299</v>
+      </c>
     </row>
-    <row r="123" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>1184</v>
       </c>
@@ -12512,8 +13050,12 @@
         <f>AVERAGE(U123:V123)</f>
         <v>37.426900584795327</v>
       </c>
+      <c r="AC123" s="8">
+        <f>_xlfn.STDEV.S(U123:V123)</f>
+        <v>15.713484026367709</v>
+      </c>
     </row>
-    <row r="124" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>1156</v>
       </c>
@@ -12599,8 +13141,12 @@
         <f>AVERAGE(U124:V124)</f>
         <v>53.508771929824569</v>
       </c>
+      <c r="AC124" s="8">
+        <f>_xlfn.STDEV.S(U124:V124)</f>
+        <v>6.2026910630398957</v>
+      </c>
     </row>
-    <row r="125" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>1186</v>
       </c>
@@ -12686,8 +13232,12 @@
         <f>AVERAGE(U125:V125)</f>
         <v>35.380116959064324</v>
       </c>
+      <c r="AC125" s="8">
+        <f>_xlfn.STDEV.S(U125:V125)</f>
+        <v>20.262124139263651</v>
+      </c>
     </row>
-    <row r="126" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>1408</v>
       </c>
@@ -12773,8 +13323,12 @@
         <f>AVERAGE(U126:V126)</f>
         <v>45.321637426900594</v>
       </c>
+      <c r="AC126" s="8">
+        <f>_xlfn.STDEV.S(U126:V126)</f>
+        <v>11.991869388543812</v>
+      </c>
     </row>
-    <row r="127" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>1158</v>
       </c>
@@ -12860,28 +13414,32 @@
         <f>AVERAGE(U127:V127)</f>
         <v>47.076023391812875</v>
       </c>
+      <c r="AC127" s="8">
+        <f>_xlfn.STDEV.S(U127:V127)</f>
+        <v>14.472945813759729</v>
+      </c>
     </row>
-    <row r="128" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A128">
-        <v>988</v>
+        <v>25</v>
       </c>
       <c r="B128">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C128">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D128">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E128">
-        <v>5000</v>
+        <v>-1</v>
       </c>
       <c r="F128">
-        <v>400</v>
+        <v>-1</v>
       </c>
       <c r="G128">
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="H128" t="s">
         <v>0</v>
@@ -12905,53 +13463,57 @@
         <v>1</v>
       </c>
       <c r="O128" t="s">
-        <v>164</v>
+        <v>101</v>
       </c>
       <c r="P128">
         <v>-1</v>
       </c>
       <c r="Q128">
-        <v>0.10657300027280581</v>
+        <v>-1</v>
       </c>
       <c r="R128">
-        <v>17</v>
+        <v>-1</v>
       </c>
       <c r="S128">
-        <v>68.658549414427569</v>
+        <v>-1</v>
       </c>
       <c r="T128">
-        <v>0.96400093014269161</v>
+        <v>-1</v>
       </c>
       <c r="U128">
-        <v>99.415204678362571</v>
+        <v>77.192982456140356</v>
       </c>
       <c r="V128">
-        <v>100</v>
+        <v>73.684210526315795</v>
       </c>
       <c r="W128" t="s">
-        <v>165</v>
+        <v>102</v>
       </c>
       <c r="X128" t="s">
-        <v>166</v>
+        <v>78</v>
       </c>
       <c r="Y128" s="12">
-        <v>127</v>
-      </c>
-      <c r="Z128" s="5">
-        <v>1</v>
-      </c>
-      <c r="AA128" s="5">
-        <v>2</v>
-      </c>
-      <c r="AB128" s="8">
+        <v>15</v>
+      </c>
+      <c r="Z128">
+        <v>1</v>
+      </c>
+      <c r="AA128">
+        <v>2</v>
+      </c>
+      <c r="AB128" s="13">
         <f>AVERAGE(U128:V128)</f>
-        <v>99.707602339181278</v>
-      </c>
-      <c r="AC128">
+        <v>75.438596491228083</v>
+      </c>
+      <c r="AC128" s="13">
+        <f>_xlfn.STDEV.S(U128:V128)</f>
+        <v>2.4810764252159565</v>
+      </c>
+      <c r="AD128">
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>1520</v>
       </c>
@@ -13037,8 +13599,12 @@
         <f>AVERAGE(U129:V129)</f>
         <v>99.707602339181278</v>
       </c>
+      <c r="AC129" s="8">
+        <f>_xlfn.STDEV.S(U129:V129)</f>
+        <v>0.41351273753599438</v>
+      </c>
     </row>
-    <row r="130" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>1887</v>
       </c>
@@ -13124,8 +13690,12 @@
         <f>AVERAGE(U130:V130)</f>
         <v>99.707602339181278</v>
       </c>
+      <c r="AC130" s="8">
+        <f>_xlfn.STDEV.S(U130:V130)</f>
+        <v>0.41351273753599438</v>
+      </c>
     </row>
-    <row r="131" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>2282</v>
       </c>
@@ -13211,8 +13781,12 @@
         <f>AVERAGE(U131:V131)</f>
         <v>99.707602339181278</v>
       </c>
+      <c r="AC131" s="8">
+        <f>_xlfn.STDEV.S(U131:V131)</f>
+        <v>0.41351273753599438</v>
+      </c>
     </row>
-    <row r="132" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>2506</v>
       </c>
@@ -13298,8 +13872,12 @@
         <f>AVERAGE(U132:V132)</f>
         <v>99.707602339181278</v>
       </c>
+      <c r="AC132" s="8">
+        <f>_xlfn.STDEV.S(U132:V132)</f>
+        <v>0.41351273753599438</v>
+      </c>
     </row>
-    <row r="133" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>1189</v>
       </c>
@@ -13385,8 +13963,12 @@
         <f>AVERAGE(U133:V133)</f>
         <v>34.795321637426902</v>
       </c>
+      <c r="AC133" s="8">
+        <f>_xlfn.STDEV.S(U133:V133)</f>
+        <v>34.321557215487395</v>
+      </c>
     </row>
-    <row r="134" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>1186</v>
       </c>
@@ -13472,8 +14054,12 @@
         <f>AVERAGE(U134:V134)</f>
         <v>35.380116959064324</v>
       </c>
+      <c r="AC134" s="8">
+        <f>_xlfn.STDEV.S(U134:V134)</f>
+        <v>20.262124139263651</v>
+      </c>
     </row>
-    <row r="135" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>1021</v>
       </c>
@@ -13559,8 +14145,12 @@
         <f>AVERAGE(U135:V135)</f>
         <v>47.953216374269005</v>
       </c>
+      <c r="AC135" s="8">
+        <f>_xlfn.STDEV.S(U135:V135)</f>
+        <v>38.043171853311335</v>
+      </c>
     </row>
-    <row r="136" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>1045</v>
       </c>
@@ -13646,8 +14236,12 @@
         <f>AVERAGE(U136:V136)</f>
         <v>54.093567251461991</v>
       </c>
+      <c r="AC136" s="8">
+        <f>_xlfn.STDEV.S(U136:V136)</f>
+        <v>46.726939341567189</v>
+      </c>
     </row>
-    <row r="137" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>1184</v>
       </c>
@@ -13733,98 +14327,106 @@
         <f>AVERAGE(U137:V137)</f>
         <v>37.426900584795327</v>
       </c>
+      <c r="AC137" s="8">
+        <f>_xlfn.STDEV.S(U137:V137)</f>
+        <v>15.713484026367709</v>
+      </c>
     </row>
-    <row r="138" spans="1:29" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A138" s="8">
-        <v>1863</v>
-      </c>
-      <c r="B138" s="8">
-        <v>1</v>
-      </c>
-      <c r="C138" s="8">
-        <v>3</v>
-      </c>
-      <c r="D138" s="8">
-        <v>3</v>
-      </c>
-      <c r="E138" s="8">
-        <v>1000</v>
-      </c>
-      <c r="F138" s="8">
-        <v>600</v>
-      </c>
-      <c r="G138" s="8">
-        <v>16.25</v>
-      </c>
-      <c r="H138" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="I138" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="J138" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="K138" s="8">
+    <row r="138" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A138">
+        <v>224</v>
+      </c>
+      <c r="B138">
+        <v>7</v>
+      </c>
+      <c r="C138">
+        <v>4</v>
+      </c>
+      <c r="D138">
+        <v>2</v>
+      </c>
+      <c r="E138">
+        <v>2000</v>
+      </c>
+      <c r="F138">
+        <v>0.4</v>
+      </c>
+      <c r="G138">
+        <v>-1</v>
+      </c>
+      <c r="H138" t="s">
+        <v>0</v>
+      </c>
+      <c r="I138" t="s">
+        <v>1</v>
+      </c>
+      <c r="J138" t="s">
+        <v>2</v>
+      </c>
+      <c r="K138">
         <v>0.35</v>
       </c>
-      <c r="L138" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="M138" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="N138" s="8">
-        <v>1</v>
-      </c>
-      <c r="O138" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="P138" s="8">
-        <v>-1</v>
-      </c>
-      <c r="Q138" s="8">
-        <v>0.15233663015660426</v>
-      </c>
-      <c r="R138" s="8">
-        <v>16</v>
-      </c>
-      <c r="S138" s="8">
-        <v>3.2968181593662313</v>
-      </c>
-      <c r="T138" s="8">
-        <v>0.99024197092243993</v>
-      </c>
-      <c r="U138" s="8">
-        <v>100</v>
-      </c>
-      <c r="V138" s="8">
-        <v>100</v>
-      </c>
-      <c r="W138" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="X138" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="Y138" s="8">
-        <v>137</v>
-      </c>
-      <c r="Z138" s="8">
-        <v>1</v>
-      </c>
-      <c r="AA138" s="8">
-        <v>1</v>
-      </c>
-      <c r="AB138" s="8">
-        <f t="shared" ref="AB130:AB161" si="1">AVERAGE(U138:V138)</f>
-        <v>100</v>
-      </c>
-      <c r="AC138" s="8">
+      <c r="L138" t="s">
+        <v>3</v>
+      </c>
+      <c r="M138" t="s">
+        <v>1</v>
+      </c>
+      <c r="N138">
+        <v>1</v>
+      </c>
+      <c r="O138" t="s">
+        <v>313</v>
+      </c>
+      <c r="P138">
+        <v>1080</v>
+      </c>
+      <c r="Q138" s="14">
+        <v>3.8844740950470136E-2</v>
+      </c>
+      <c r="R138">
+        <v>44</v>
+      </c>
+      <c r="S138">
+        <v>19.313113661046593</v>
+      </c>
+      <c r="T138">
+        <v>0.979917810676321</v>
+      </c>
+      <c r="U138">
+        <v>77.777777777777771</v>
+      </c>
+      <c r="V138">
+        <v>94.736842105263165</v>
+      </c>
+      <c r="W138" t="s">
+        <v>314</v>
+      </c>
+      <c r="X138" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y138" s="12">
+        <v>89</v>
+      </c>
+      <c r="Z138" s="5">
+        <v>1</v>
+      </c>
+      <c r="AA138" s="5">
+        <v>2</v>
+      </c>
+      <c r="AB138" s="13">
+        <f>AVERAGE(U138:V138)</f>
+        <v>86.257309941520475</v>
+      </c>
+      <c r="AC138" s="13">
+        <f>_xlfn.STDEV.S(U138:V138)</f>
+        <v>11.991869388543797</v>
+      </c>
+      <c r="AD138">
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>3319</v>
       </c>
@@ -13907,11 +14509,15 @@
         <v>1</v>
       </c>
       <c r="AB139" s="8">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(U139:V139)</f>
         <v>100</v>
       </c>
+      <c r="AC139" s="8">
+        <f>_xlfn.STDEV.S(U139:V139)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="140" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>3491</v>
       </c>
@@ -13994,11 +14600,15 @@
         <v>1</v>
       </c>
       <c r="AB140" s="8">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(U140:V140)</f>
         <v>100</v>
       </c>
+      <c r="AC140" s="8">
+        <f>_xlfn.STDEV.S(U140:V140)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="141" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>3493</v>
       </c>
@@ -14081,11 +14691,15 @@
         <v>1</v>
       </c>
       <c r="AB141" s="8">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(U141:V141)</f>
         <v>100</v>
       </c>
+      <c r="AC141" s="8">
+        <f>_xlfn.STDEV.S(U141:V141)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="142" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>3683</v>
       </c>
@@ -14168,11 +14782,15 @@
         <v>1</v>
       </c>
       <c r="AB142" s="8">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(U142:V142)</f>
         <v>100</v>
       </c>
+      <c r="AC142" s="8">
+        <f>_xlfn.STDEV.S(U142:V142)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="143" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>1334</v>
       </c>
@@ -14255,11 +14873,15 @@
         <v>1</v>
       </c>
       <c r="AB143" s="8">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(U143:V143)</f>
         <v>47.953216374269012</v>
       </c>
+      <c r="AC143" s="8">
+        <f>_xlfn.STDEV.S(U143:V143)</f>
+        <v>0.82702547507197877</v>
+      </c>
     </row>
-    <row r="144" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>1085</v>
       </c>
@@ -14342,11 +14964,15 @@
         <v>1</v>
       </c>
       <c r="AB144" s="8">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(U144:V144)</f>
         <v>49.707602339181292</v>
       </c>
+      <c r="AC144" s="8">
+        <f>_xlfn.STDEV.S(U144:V144)</f>
+        <v>3.308101900287935</v>
+      </c>
     </row>
-    <row r="145" spans="1:28" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>1276</v>
       </c>
@@ -14429,11 +15055,15 @@
         <v>1</v>
       </c>
       <c r="AB145" s="8">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(U145:V145)</f>
         <v>42.397660818713462</v>
       </c>
+      <c r="AC145" s="8">
+        <f>_xlfn.STDEV.S(U145:V145)</f>
+        <v>15.299971288831703</v>
+      </c>
     </row>
-    <row r="146" spans="1:28" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>1308</v>
       </c>
@@ -14516,11 +15146,15 @@
         <v>1</v>
       </c>
       <c r="AB146" s="8">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(U146:V146)</f>
         <v>51.461988304093573</v>
       </c>
+      <c r="AC146" s="8">
+        <f>_xlfn.STDEV.S(U146:V146)</f>
+        <v>5.7891783255038911</v>
+      </c>
     </row>
-    <row r="147" spans="1:28" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>1303</v>
       </c>
@@ -14603,11 +15237,15 @@
         <v>1</v>
       </c>
       <c r="AB147" s="8">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(U147:V147)</f>
         <v>51.169590643274859</v>
       </c>
+      <c r="AC147" s="8">
+        <f>_xlfn.STDEV.S(U147:V147)</f>
+        <v>12.818894863615757</v>
+      </c>
     </row>
-    <row r="148" spans="1:28" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>1863</v>
       </c>
@@ -14690,11 +15328,15 @@
         <v>2</v>
       </c>
       <c r="AB148" s="8">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(U148:V148)</f>
         <v>100</v>
       </c>
+      <c r="AC148" s="8">
+        <f>_xlfn.STDEV.S(U148:V148)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="149" spans="1:28" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>3319</v>
       </c>
@@ -14777,11 +15419,15 @@
         <v>2</v>
       </c>
       <c r="AB149" s="8">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(U149:V149)</f>
         <v>100</v>
       </c>
+      <c r="AC149" s="8">
+        <f>_xlfn.STDEV.S(U149:V149)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="150" spans="1:28" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>3491</v>
       </c>
@@ -14864,11 +15510,15 @@
         <v>2</v>
       </c>
       <c r="AB150" s="8">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(U150:V150)</f>
         <v>100</v>
       </c>
+      <c r="AC150" s="8">
+        <f>_xlfn.STDEV.S(U150:V150)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="151" spans="1:28" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>3493</v>
       </c>
@@ -14951,11 +15601,15 @@
         <v>2</v>
       </c>
       <c r="AB151" s="8">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(U151:V151)</f>
         <v>100</v>
       </c>
+      <c r="AC151" s="8">
+        <f>_xlfn.STDEV.S(U151:V151)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="152" spans="1:28" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>3683</v>
       </c>
@@ -15038,11 +15692,15 @@
         <v>2</v>
       </c>
       <c r="AB152" s="8">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(U152:V152)</f>
         <v>100</v>
       </c>
+      <c r="AC152" s="8">
+        <f>_xlfn.STDEV.S(U152:V152)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="153" spans="1:28" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>1225</v>
       </c>
@@ -15125,11 +15783,15 @@
         <v>2</v>
       </c>
       <c r="AB153" s="8">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(U153:V153)</f>
         <v>41.520467836257303</v>
       </c>
+      <c r="AC153" s="8">
+        <f>_xlfn.STDEV.S(U153:V153)</f>
+        <v>36.389120903167367</v>
+      </c>
     </row>
-    <row r="154" spans="1:28" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>1333</v>
       </c>
@@ -15212,11 +15874,15 @@
         <v>2</v>
       </c>
       <c r="AB154" s="8">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(U154:V154)</f>
         <v>52.046783625730995</v>
       </c>
+      <c r="AC154" s="8">
+        <f>_xlfn.STDEV.S(U154:V154)</f>
+        <v>43.832350178815233</v>
+      </c>
     </row>
-    <row r="155" spans="1:28" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>1057</v>
       </c>
@@ -15299,11 +15965,15 @@
         <v>2</v>
       </c>
       <c r="AB155" s="8">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(U155:V155)</f>
         <v>45.029239766081872</v>
       </c>
+      <c r="AC155" s="8">
+        <f>_xlfn.STDEV.S(U155:V155)</f>
+        <v>26.464815202303534</v>
+      </c>
     </row>
-    <row r="156" spans="1:28" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>1192</v>
       </c>
@@ -15386,11 +16056,15 @@
         <v>2</v>
       </c>
       <c r="AB156" s="8">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(U156:V156)</f>
         <v>46.491228070175445</v>
       </c>
+      <c r="AC156" s="8">
+        <f>_xlfn.STDEV.S(U156:V156)</f>
+        <v>28.532378889983505</v>
+      </c>
     </row>
-    <row r="157" spans="1:28" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>1164</v>
       </c>
@@ -15473,11 +16147,15 @@
         <v>2</v>
       </c>
       <c r="AB157" s="8">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(U157:V157)</f>
         <v>47.076023391812868</v>
       </c>
+      <c r="AC157" s="8">
+        <f>_xlfn.STDEV.S(U157:V157)</f>
+        <v>29.359404365055472</v>
+      </c>
     </row>
-    <row r="158" spans="1:28" s="8" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:29" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158" s="8">
         <v>1536</v>
       </c>
@@ -15560,11 +16238,15 @@
         <v>1</v>
       </c>
       <c r="AB158" s="8">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(U158:V158)</f>
         <v>78.94736842105263</v>
       </c>
+      <c r="AC158" s="8">
+        <f>_xlfn.STDEV.S(U158:V158)</f>
+        <v>29.772917102591492</v>
+      </c>
     </row>
-    <row r="159" spans="1:28" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>3330</v>
       </c>
@@ -15647,11 +16329,15 @@
         <v>1</v>
       </c>
       <c r="AB159" s="8">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(U159:V159)</f>
         <v>76.023391812865498</v>
       </c>
+      <c r="AC159" s="8">
+        <f>_xlfn.STDEV.S(U159:V159)</f>
+        <v>33.08101900287943</v>
+      </c>
     </row>
-    <row r="160" spans="1:28" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>3864</v>
       </c>
@@ -15734,11 +16420,15 @@
         <v>1</v>
       </c>
       <c r="AB160" s="8">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(U160:V160)</f>
         <v>89.181286549707607</v>
       </c>
+      <c r="AC160" s="8">
+        <f>_xlfn.STDEV.S(U160:V160)</f>
+        <v>14.472945813759667</v>
+      </c>
     </row>
-    <row r="161" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>3384</v>
       </c>
@@ -15821,11 +16511,15 @@
         <v>1</v>
       </c>
       <c r="AB161" s="8">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(U161:V161)</f>
         <v>88.888888888888886</v>
       </c>
+      <c r="AC161" s="8">
+        <f>_xlfn.STDEV.S(U161:V161)</f>
+        <v>14.059433076223748</v>
+      </c>
     </row>
-    <row r="162" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>3696</v>
       </c>
@@ -15908,11 +16602,15 @@
         <v>1</v>
       </c>
       <c r="AB162" s="8">
-        <f t="shared" ref="AB162:AB177" si="2">AVERAGE(U162:V162)</f>
+        <f>AVERAGE(U162:V162)</f>
         <v>88.888888888888886</v>
       </c>
+      <c r="AC162" s="8">
+        <f>_xlfn.STDEV.S(U162:V162)</f>
+        <v>14.059433076223748</v>
+      </c>
     </row>
-    <row r="163" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>1338</v>
       </c>
@@ -15995,11 +16693,15 @@
         <v>1</v>
       </c>
       <c r="AB163" s="8">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(U163:V163)</f>
         <v>45.321637426900594</v>
       </c>
+      <c r="AC163" s="8">
+        <f>_xlfn.STDEV.S(U163:V163)</f>
+        <v>4.5486401128959137</v>
+      </c>
     </row>
-    <row r="164" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>1366</v>
       </c>
@@ -16082,11 +16784,15 @@
         <v>1</v>
       </c>
       <c r="AB164" s="8">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(U164:V164)</f>
         <v>45.906432748538016</v>
       </c>
+      <c r="AC164" s="8">
+        <f>_xlfn.STDEV.S(U164:V164)</f>
+        <v>5.3756655879678972</v>
+      </c>
     </row>
-    <row r="165" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>1199</v>
       </c>
@@ -16169,11 +16875,15 @@
         <v>1</v>
       </c>
       <c r="AB165" s="8">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(U165:V165)</f>
         <v>59.064327485380119</v>
       </c>
+      <c r="AC165" s="8">
+        <f>_xlfn.STDEV.S(U165:V165)</f>
+        <v>1.6540509501439626</v>
+      </c>
     </row>
-    <row r="166" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>1316</v>
       </c>
@@ -16256,11 +16966,15 @@
         <v>1</v>
       </c>
       <c r="AB166" s="8">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(U166:V166)</f>
         <v>47.953216374269012</v>
       </c>
+      <c r="AC166" s="8">
+        <f>_xlfn.STDEV.S(U166:V166)</f>
+        <v>23.156713302015579</v>
+      </c>
     </row>
-    <row r="167" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>1286</v>
       </c>
@@ -16343,11 +17057,15 @@
         <v>1</v>
       </c>
       <c r="AB167" s="8">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(U167:V167)</f>
         <v>64.035087719298247</v>
       </c>
+      <c r="AC167" s="8">
+        <f>_xlfn.STDEV.S(U167:V167)</f>
+        <v>1.2405382126079683</v>
+      </c>
     </row>
-    <row r="168" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>1592</v>
       </c>
@@ -16430,11 +17148,15 @@
         <v>2</v>
       </c>
       <c r="AB168" s="8">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(U168:V168)</f>
         <v>98.245614035087726</v>
       </c>
+      <c r="AC168" s="8">
+        <f>_xlfn.STDEV.S(U168:V168)</f>
+        <v>2.4810764252159565</v>
+      </c>
     </row>
-    <row r="169" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>1982</v>
       </c>
@@ -16517,11 +17239,15 @@
         <v>2</v>
       </c>
       <c r="AB169" s="8">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(U169:V169)</f>
         <v>98.245614035087726</v>
       </c>
+      <c r="AC169" s="8">
+        <f>_xlfn.STDEV.S(U169:V169)</f>
+        <v>2.4810764252159565</v>
+      </c>
     </row>
-    <row r="170" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>4140</v>
       </c>
@@ -16604,11 +17330,15 @@
         <v>2</v>
       </c>
       <c r="AB170" s="8">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(U170:V170)</f>
         <v>98.245614035087726</v>
       </c>
+      <c r="AC170" s="8">
+        <f>_xlfn.STDEV.S(U170:V170)</f>
+        <v>2.4810764252159565</v>
+      </c>
     </row>
-    <row r="171" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>1786</v>
       </c>
@@ -16657,7 +17387,7 @@
       <c r="P171">
         <v>-1</v>
       </c>
-      <c r="Q171">
+      <c r="Q171" s="14">
         <v>0.29532003567509157</v>
       </c>
       <c r="R171">
@@ -16690,15 +17420,19 @@
       <c r="AA171" s="5">
         <v>2</v>
       </c>
-      <c r="AB171" s="8">
-        <f t="shared" si="2"/>
+      <c r="AB171" s="13">
+        <f>AVERAGE(U171:V171)</f>
         <v>98.538011695906434</v>
       </c>
-      <c r="AC171">
+      <c r="AC171" s="13">
+        <f>_xlfn.STDEV.S(U171:V171)</f>
+        <v>2.0675636876799621</v>
+      </c>
+      <c r="AD171">
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>1932</v>
       </c>
@@ -16781,11 +17515,15 @@
         <v>2</v>
       </c>
       <c r="AB172" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="AB162:AB177" si="2">AVERAGE(U172:V172)</f>
         <v>96.491228070175453</v>
       </c>
+      <c r="AC172" s="8">
+        <f t="shared" ref="AC131:AC177" si="3">_xlfn.STDEV.S(U172:V172)</f>
+        <v>2.4810764252159565</v>
+      </c>
     </row>
-    <row r="173" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>1147</v>
       </c>
@@ -16871,8 +17609,12 @@
         <f t="shared" si="2"/>
         <v>49.415204678362571</v>
       </c>
+      <c r="AC173" s="8">
+        <f t="shared" si="3"/>
+        <v>47.553964816639173</v>
+      </c>
     </row>
-    <row r="174" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>1315</v>
       </c>
@@ -16958,8 +17700,12 @@
         <f t="shared" si="2"/>
         <v>47.66081871345029</v>
       </c>
+      <c r="AC174" s="8">
+        <f t="shared" si="3"/>
+        <v>37.629659115775333</v>
+      </c>
     </row>
-    <row r="175" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>1091</v>
       </c>
@@ -17045,8 +17791,12 @@
         <f t="shared" si="2"/>
         <v>47.953216374269005</v>
       </c>
+      <c r="AC175" s="8">
+        <f t="shared" si="3"/>
+        <v>38.043171853311335</v>
+      </c>
     </row>
-    <row r="176" spans="1:29" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>1228</v>
       </c>
@@ -17132,8 +17882,12 @@
         <f t="shared" si="2"/>
         <v>49.415204678362571</v>
       </c>
+      <c r="AC176" s="8">
+        <f t="shared" si="3"/>
+        <v>40.110735540991293</v>
+      </c>
     </row>
-    <row r="177" spans="1:28" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>1059</v>
       </c>
@@ -17219,16 +17973,20 @@
         <f t="shared" si="2"/>
         <v>50.000000000000007</v>
       </c>
+      <c r="AC177" s="8">
+        <f t="shared" si="3"/>
+        <v>33.494531740415411</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AC177">
-    <filterColumn colId="28">
+  <autoFilter ref="A1:AD177" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="29">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
       </customFilters>
     </filterColumn>
-    <sortState ref="A6:AC137">
-      <sortCondition ref="Y1:Y177"/>
+    <sortState ref="A4:AD171">
+      <sortCondition ref="C1:C177"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>